<commit_message>
Stable RO.ACT et RO.FOU
Correction format date dans JDD Generator.addInfoVersion
 Suppression du screenshot sur msg = "Fin de la  vérification des
valeurs en Base de Données"
 Ajout des liens vers screenshot
 Ajout du ctrl varchar dans CheckTypeInDATA.run()
 Ajout de fonction dans InfoBDD
 Traitement des memo dans RO.FOU
 en cours traitement de ADR
</commit_message>
<xml_diff>
--- a/TNR/TCGenerator.xlsx
+++ b/TNR/TCGenerator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="48" windowWidth="22116" windowHeight="11400" activeTab="1"/>
+    <workbookView xWindow="288" yWindow="48" windowWidth="22116" windowHeight="11400"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez moi" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="102">
   <si>
     <t>ID_CODGES</t>
   </si>
@@ -303,6 +303,30 @@
   </si>
   <si>
     <t>TEXTES COMMANDE</t>
+  </si>
+  <si>
+    <t>Ne pas faire de setText sur la clé PRI</t>
+  </si>
+  <si>
+    <t>Dans le cas des KW.searchWithHelper, vérifier si le 2e paramètre 'btnXpath' et le 3e paramètre 'inputSearchName' sont std sinon les renseigner</t>
+  </si>
+  <si>
+    <t>REC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ne pas oublier </t>
+  </si>
+  <si>
+    <t>input_Filtre_Grille</t>
+  </si>
+  <si>
+    <t>td_Grille</t>
+  </si>
+  <si>
+    <t>$FILTREGRILLE$ID de la clé primaire</t>
+  </si>
+  <si>
+    <t>$TDGRILLE$ID de la clé primaire</t>
   </si>
 </sst>
 </file>
@@ -411,7 +435,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -431,6 +455,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,184 +478,7 @@
     <cellStyle name="Normal 8" xfId="11"/>
     <cellStyle name="Normal 9" xfId="12"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <strike val="0"/>
@@ -936,14 +786,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A6:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:5">
+      <c r="A6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -952,9 +858,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1296,6 +1202,7 @@
       <c r="B13" s="14" t="s">
         <v>59</v>
       </c>
+      <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
         <v>54</v>
       </c>
@@ -1304,7 +1211,7 @@
         <v>KW.scrollAndSetText(myJDD,"ST_CODCOM")</v>
       </c>
       <c r="G13" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(D13),"",VLOOKUP(D13,TAG_List,4,FALSE)&amp;B13&amp;VLOOKUP(D13,TAG_List,5,FALSE))</f>
         <v>KW.searchWithHelper(myJDD, "ST_CODCOM","","")</v>
       </c>
       <c r="H13" s="15" t="str">
@@ -2326,10 +2233,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:H1048576">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$D1="block"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>$D1="onglet"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2351,7 +2258,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2533,7 +2440,7 @@
       <c r="C7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="15" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="6" t="s">

</xml_diff>

<commit_message>
Correction de JDD et reprise
KW.verifyDateValue
KW.verifyDateText
simplification des LEC correspondant
Prise en compte dans TCGenerator
</commit_message>
<xml_diff>
--- a/TNR/TCGenerator.xlsx
+++ b/TNR/TCGenerator.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="48" windowWidth="22116" windowHeight="11400"/>
+    <workbookView xWindow="288" yWindow="48" windowWidth="22116" windowHeight="11400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez moi" sheetId="5" r:id="rId1"/>
-    <sheet name="Generator" sheetId="1" r:id="rId2"/>
-    <sheet name="TAG" sheetId="2" r:id="rId3"/>
+    <sheet name="Version" sheetId="6" r:id="rId2"/>
+    <sheet name="Generator" sheetId="1" r:id="rId3"/>
+    <sheet name="TAG" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Step">Generator!$A:$J</definedName>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="110">
   <si>
     <t>ID_CODGES</t>
   </si>
@@ -327,6 +328,30 @@
   </si>
   <si>
     <t>$TDGRILLE$ID de la clé primaire</t>
+  </si>
+  <si>
+    <t>inputDate</t>
+  </si>
+  <si>
+    <t>KW.verifyDateValue(myJDD,"</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Auteur</t>
+  </si>
+  <si>
+    <t>Objet</t>
+  </si>
+  <si>
+    <t>JM Lafarge</t>
+  </si>
+  <si>
+    <t>Création</t>
+  </si>
+  <si>
+    <t>Ajout inputDate</t>
   </si>
 </sst>
 </file>
@@ -375,7 +400,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,13 +431,34 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -435,7 +481,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -458,6 +504,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,7 +837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A6:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -856,11 +905,110 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C29:C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="78.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="23">
+        <v>45012</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="23">
+        <v>45004</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2253,12 +2401,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2407,7 +2555,7 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" t="s">
+      <c r="A6" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2430,45 +2578,45 @@
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:9" s="5" customFormat="1">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:9" s="15" customFormat="1">
+      <c r="A7" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="1:9" s="5" customFormat="1">
+      <c r="A8" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D8" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>46</v>
@@ -2480,63 +2628,87 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Création de my.TO et autres
</commit_message>
<xml_diff>
--- a/TNR/TCGenerator.xlsx
+++ b/TNR/TCGenerator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="48" windowWidth="22116" windowHeight="11400" activeTab="3"/>
+    <workbookView xWindow="288" yWindow="48" windowWidth="22116" windowHeight="11400" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez moi" sheetId="5" r:id="rId1"/>
@@ -135,12 +135,6 @@
     <t xml:space="preserve"> --&gt; pas d'action en modification</t>
   </si>
   <si>
-    <t>MYLOG.addSTEPBLOCK("</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MYLOG.addSTEPGRP("ONGLET </t>
-  </si>
-  <si>
     <t>")</t>
   </si>
   <si>
@@ -358,6 +352,12 @@
   </si>
   <si>
     <t>KW.scrollAndSetDate(myJDD, "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TNRResult.addSTEPGRP("ONGLET </t>
+  </si>
+  <si>
+    <t>TNRResult.addSTEPBLOCK("</t>
   </si>
 </sst>
 </file>
@@ -859,7 +859,7 @@
         <v>27</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -867,41 +867,41 @@
         <v>27</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>98</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>99</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -926,13 +926,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>104</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -940,10 +940,10 @@
         <v>45012</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -951,10 +951,10 @@
         <v>45004</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>107</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1012,7 +1012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
@@ -1038,7 +1038,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1067,7 +1067,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="15" t="s">
@@ -1076,15 +1076,15 @@
       <c r="E2" s="4"/>
       <c r="F2" t="str">
         <f t="shared" ref="F2" si="0">IF(ISBLANK(D2),"",VLOOKUP(D2,TAG_List,2,FALSE)&amp;B2&amp;VLOOKUP(D2,TAG_List,3,FALSE))</f>
-        <v>MYLOG.addSTEPGRP("ONGLET FOURNISSEUR")</v>
+        <v>TNRResult.addSTEPGRP("ONGLET FOURNISSEUR")</v>
       </c>
       <c r="G2" s="5" t="str">
         <f t="shared" ref="G2" si="1">IF(ISBLANK(D2),"",VLOOKUP(D2,TAG_List,4,FALSE)&amp;B2&amp;VLOOKUP(D2,TAG_List,5,FALSE))</f>
-        <v>MYLOG.addSTEPGRP("ONGLET FOURNISSEUR")</v>
+        <v>TNRResult.addSTEPGRP("ONGLET FOURNISSEUR")</v>
       </c>
       <c r="H2" t="str">
         <f t="shared" ref="H2" si="2">IF(ISBLANK(D2),"",VLOOKUP(D2,TAG_List,6,FALSE)&amp;B2&amp;VLOOKUP(D2,TAG_List,7,FALSE))</f>
-        <v>MYLOG.addSTEPGRP("ONGLET FOURNISSEUR")</v>
+        <v>TNRResult.addSTEPGRP("ONGLET FOURNISSEUR")</v>
       </c>
       <c r="I2" s="8" t="str">
         <f t="shared" ref="I2" si="3">IF(OR(D2="tab",D2="tabselected"),B2&amp;VLOOKUP(D2,TAG_List,8,FALSE),"")</f>
@@ -1107,10 +1107,10 @@
     </row>
     <row r="4" spans="1:10" s="8" customFormat="1">
       <c r="B4" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>8</v>
@@ -1140,10 +1140,10 @@
     <row r="5" spans="1:10" s="2" customFormat="1">
       <c r="A5" s="8"/>
       <c r="B5" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>9</v>
@@ -1182,7 +1182,7 @@
     <row r="7" spans="1:10" s="2" customFormat="1">
       <c r="A7" s="8"/>
       <c r="B7" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="15" t="s">
@@ -1245,7 +1245,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F9" s="15" t="str">
         <f t="shared" si="5"/>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="B11" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>3</v>
@@ -1354,11 +1354,11 @@
     </row>
     <row r="13" spans="1:10">
       <c r="B13" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F13" s="15" t="str">
         <f t="shared" si="5"/>
@@ -1383,7 +1383,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="B14" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>11</v>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="15" spans="1:10" s="15" customFormat="1">
       <c r="B15" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>12</v>
@@ -1449,7 +1449,7 @@
     </row>
     <row r="17" spans="2:10">
       <c r="B17" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>2</v>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="19" spans="2:10">
       <c r="B19" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>2</v>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="21" spans="2:10">
       <c r="B21" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>2</v>
@@ -1593,22 +1593,22 @@
     </row>
     <row r="23" spans="2:10">
       <c r="B23" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="15" t="str">
         <f t="shared" si="5"/>
-        <v>MYLOG.addSTEPGRP("ONGLET COMMANDE")</v>
+        <v>TNRResult.addSTEPGRP("ONGLET COMMANDE")</v>
       </c>
       <c r="G23" s="15" t="str">
         <f t="shared" si="6"/>
-        <v>MYLOG.addSTEPGRP("ONGLET COMMANDE")</v>
+        <v>TNRResult.addSTEPGRP("ONGLET COMMANDE")</v>
       </c>
       <c r="H23" s="15" t="str">
         <f t="shared" si="7"/>
-        <v>MYLOG.addSTEPGRP("ONGLET COMMANDE")</v>
+        <v>TNRResult.addSTEPGRP("ONGLET COMMANDE")</v>
       </c>
       <c r="I23" s="18" t="str">
         <f t="shared" si="8"/>
@@ -1625,10 +1625,10 @@
     </row>
     <row r="25" spans="2:10">
       <c r="B25" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>8</v>
@@ -1656,10 +1656,10 @@
     </row>
     <row r="26" spans="2:10">
       <c r="B26" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>9</v>
@@ -1691,7 +1691,7 @@
     </row>
     <row r="28" spans="2:10">
       <c r="B28" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>2</v>
@@ -1719,10 +1719,10 @@
     </row>
     <row r="29" spans="2:10">
       <c r="B29" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F29" s="15" t="str">
         <f t="shared" si="5"/>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="30" spans="2:10">
       <c r="B30" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>11</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>2</v>
@@ -1803,10 +1803,10 @@
     </row>
     <row r="32" spans="2:10">
       <c r="B32" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F32" s="15" t="str">
         <f t="shared" si="5"/>
@@ -1831,7 +1831,7 @@
     </row>
     <row r="33" spans="2:10">
       <c r="B33" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>11</v>
@@ -1859,10 +1859,10 @@
     </row>
     <row r="34" spans="2:10">
       <c r="B34" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F34" s="15" t="str">
         <f t="shared" si="5"/>
@@ -1887,7 +1887,7 @@
     </row>
     <row r="35" spans="2:10">
       <c r="B35" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>11</v>
@@ -1915,10 +1915,10 @@
     </row>
     <row r="36" spans="2:10">
       <c r="B36" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F36" s="15" t="str">
         <f t="shared" si="5"/>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="37" spans="2:10">
       <c r="B37" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D37" s="15" t="s">
         <v>11</v>
@@ -1971,10 +1971,10 @@
     </row>
     <row r="38" spans="2:10">
       <c r="B38" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F38" s="15" t="str">
         <f t="shared" si="5"/>
@@ -1999,7 +1999,7 @@
     </row>
     <row r="39" spans="2:10">
       <c r="B39" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>11</v>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="40" spans="2:10">
       <c r="B40" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>2</v>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="41" spans="2:10">
       <c r="B41" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>3</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="42" spans="2:10" s="15" customFormat="1">
       <c r="B42" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>12</v>
@@ -2093,7 +2093,7 @@
     </row>
     <row r="43" spans="2:10">
       <c r="B43" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>2</v>
@@ -2121,7 +2121,7 @@
     </row>
     <row r="44" spans="2:10">
       <c r="B44" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>2</v>
@@ -2149,7 +2149,7 @@
     </row>
     <row r="45" spans="2:10">
       <c r="B45" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>2</v>
@@ -2177,7 +2177,7 @@
     </row>
     <row r="46" spans="2:10">
       <c r="B46" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D46" s="15" t="s">
         <v>2</v>
@@ -2205,7 +2205,7 @@
     </row>
     <row r="47" spans="2:10">
       <c r="B47" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D47" s="15" t="s">
         <v>2</v>
@@ -2233,7 +2233,7 @@
     </row>
     <row r="48" spans="2:10">
       <c r="B48" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D48" s="15" t="s">
         <v>2</v>
@@ -2261,7 +2261,7 @@
     </row>
     <row r="49" spans="2:10">
       <c r="B49" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D49" s="15" t="s">
         <v>3</v>
@@ -2293,22 +2293,22 @@
     </row>
     <row r="51" spans="2:10">
       <c r="B51" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D51" s="15" t="s">
         <v>7</v>
       </c>
       <c r="F51" s="15" t="str">
         <f t="shared" si="5"/>
-        <v>MYLOG.addSTEPGRP("ONGLET NOTES")</v>
+        <v>TNRResult.addSTEPGRP("ONGLET NOTES")</v>
       </c>
       <c r="G51" s="15" t="str">
         <f t="shared" si="6"/>
-        <v>MYLOG.addSTEPGRP("ONGLET NOTES")</v>
+        <v>TNRResult.addSTEPGRP("ONGLET NOTES")</v>
       </c>
       <c r="H51" s="15" t="str">
         <f t="shared" si="7"/>
-        <v>MYLOG.addSTEPGRP("ONGLET NOTES")</v>
+        <v>TNRResult.addSTEPGRP("ONGLET NOTES")</v>
       </c>
       <c r="I51" s="18" t="str">
         <f t="shared" si="8"/>
@@ -2325,10 +2325,10 @@
     </row>
     <row r="53" spans="2:10">
       <c r="B53" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D53" s="15" t="s">
         <v>8</v>
@@ -2356,10 +2356,10 @@
     </row>
     <row r="54" spans="2:10">
       <c r="B54" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D54" s="15" t="s">
         <v>9</v>
@@ -2411,8 +2411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2460,23 +2460,23 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>38</v>
+      <c r="B2" s="15" t="s">
+        <v>110</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>110</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>110</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H2" s="6"/>
     </row>
@@ -2484,23 +2484,23 @@
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="H3" s="6"/>
     </row>
@@ -2509,22 +2509,22 @@
         <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="9" t="s">
@@ -2536,22 +2536,22 @@
         <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>25</v>
@@ -2565,70 +2565,70 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:9" s="15" customFormat="1">
       <c r="A7" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:9" s="5" customFormat="1">
       <c r="A8" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="15" t="s">
+      <c r="F8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="G8" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H8" s="6"/>
     </row>
@@ -2649,10 +2649,10 @@
         <v>36</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H9" s="6"/>
     </row>
@@ -2661,22 +2661,22 @@
         <v>3</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="G10" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H10" s="6"/>
     </row>
@@ -2685,37 +2685,37 @@
         <v>22</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>